<commit_message>
Added Log4J logging and few testcases
</commit_message>
<xml_diff>
--- a/src/main/resources/data/TestData.xlsx
+++ b/src/main/resources/data/TestData.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abishiek/Studies/IIT Roorkie/selenium-ui-automation/src/main/resources/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1677AAE-427F-2941-B7DF-7317578860CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA0BA310-DDD8-B648-BE6C-1E65FD6B59DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16040" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TC00001" sheetId="1" r:id="rId1"/>
+    <sheet name="TC00002" sheetId="2" r:id="rId2"/>
+    <sheet name="TC00003" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -25,19 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>menu1</t>
-  </si>
-  <si>
-    <t>menu2</t>
-  </si>
-  <si>
-    <t>menu3</t>
-  </si>
-  <si>
-    <t>menu4</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>About</t>
   </si>
@@ -49,13 +39,103 @@
   </si>
   <si>
     <t>Logout</t>
+  </si>
+  <si>
+    <t>SUPPORT_URL</t>
+  </si>
+  <si>
+    <t>https://opensource-demo.orangehrmlive.com/web/index.php/help/support</t>
+  </si>
+  <si>
+    <t>CHANGE_PASSWORD_URL</t>
+  </si>
+  <si>
+    <t>https://opensource-demo.orangehrmlive.com/web/index.php/pim/updatePassword</t>
+  </si>
+  <si>
+    <t>MENU1</t>
+  </si>
+  <si>
+    <t>MENU2</t>
+  </si>
+  <si>
+    <t>MENU3</t>
+  </si>
+  <si>
+    <t>MENU4</t>
+  </si>
+  <si>
+    <t>SIDEMENU1</t>
+  </si>
+  <si>
+    <t>SIDEMENU2</t>
+  </si>
+  <si>
+    <t>SIDEMENU3</t>
+  </si>
+  <si>
+    <t>SIDEMENU4</t>
+  </si>
+  <si>
+    <t>SIDEMENU5</t>
+  </si>
+  <si>
+    <t>SIDEMENU6</t>
+  </si>
+  <si>
+    <t>SIDEMENU7</t>
+  </si>
+  <si>
+    <t>SIDEMENU8</t>
+  </si>
+  <si>
+    <t>SIDEMENU9</t>
+  </si>
+  <si>
+    <t>SIDEMENU10</t>
+  </si>
+  <si>
+    <t>SIDEMENU11</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>PIM</t>
+  </si>
+  <si>
+    <t>Leave</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Recruitment</t>
+  </si>
+  <si>
+    <t>My Info</t>
+  </si>
+  <si>
+    <t>Performance</t>
+  </si>
+  <si>
+    <t>Dashboard</t>
+  </si>
+  <si>
+    <t>Directory</t>
+  </si>
+  <si>
+    <t>Maintenance</t>
+  </si>
+  <si>
+    <t>Buzz</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -66,6 +146,36 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -100,14 +210,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -323,8 +439,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -337,34 +453,160 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D440111B-6BD7-8445-A451-EB794F99CC46}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="64.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="71.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{8EA77F2E-34E9-5745-9372-D060DB794123}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C27E7A9F-3BDB-5544-BF9C-5426D06E1F1C}">
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="10" max="11" width="12.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>